<commit_message>
changes to xl and codebook
</commit_message>
<xml_diff>
--- a/week4 assignment labeling.xlsx
+++ b/week4 assignment labeling.xlsx
@@ -803,8 +803,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -888,7 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -922,6 +924,7 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -955,6 +958,7 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -1696,7 +1700,7 @@
   <dimension ref="B2:P85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:P2"/>
+      <selection activeCell="P5" sqref="P5:P85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1802,8 +1806,8 @@
         <v>Mean_of_X_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P5" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-mean()-X                      New Column Name: Mean_of_X_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-mean()-X     &gt;&gt;     Mean_of_X_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="6" spans="2:16">
@@ -1837,8 +1841,8 @@
         <v>Mean_of_Y_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P6" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-mean()-Y                      New Column Name: Mean_of_Y_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-mean()-Y     &gt;&gt;     Mean_of_Y_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="7" spans="2:16">
@@ -1872,8 +1876,8 @@
         <v>Mean_of_Z_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P7" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-mean()-Z                      New Column Name: Mean_of_Z_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-mean()-Z     &gt;&gt;     Mean_of_Z_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="8" spans="2:16">
@@ -1907,8 +1911,8 @@
         <v>MeanFreq_of_X_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P8" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-meanFreq()-X                      New Column Name: MeanFreq_of_X_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-meanFreq()-X     &gt;&gt;     MeanFreq_of_X_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="9" spans="2:16">
@@ -1942,8 +1946,8 @@
         <v>MeanFreq_of_Y_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P9" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-meanFreq()-Y                      New Column Name: MeanFreq_of_Y_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-meanFreq()-Y     &gt;&gt;     MeanFreq_of_Y_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="10" spans="2:16">
@@ -1977,8 +1981,8 @@
         <v>MeanFreq_of_Z_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P10" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-meanFreq()-Z                      New Column Name: MeanFreq_of_Z_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-meanFreq()-Z     &gt;&gt;     MeanFreq_of_Z_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="11" spans="2:16">
@@ -2012,8 +2016,8 @@
         <v>StdDev_of_X_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P11" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-std()-X                      New Column Name: StdDev_of_X_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-std()-X     &gt;&gt;     StdDev_of_X_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="12" spans="2:16">
@@ -2047,8 +2051,8 @@
         <v>StdDev_of_Y_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P12" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-std()-Y                      New Column Name: StdDev_of_Y_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-std()-Y     &gt;&gt;     StdDev_of_Y_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="13" spans="2:16">
@@ -2082,8 +2086,8 @@
         <v>StdDev_of_Z_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P13" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccJerk-std()-Z                      New Column Name: StdDev_of_Z_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccJerk-std()-Z     &gt;&gt;     StdDev_of_Z_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="14" spans="2:16">
@@ -2117,8 +2121,8 @@
         <v>Mean_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P14" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyAccJerkMag-mean()                      New Column Name: Mean_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyAccJerkMag-mean()     &gt;&gt;     Mean_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="15" spans="2:16">
@@ -2152,8 +2156,8 @@
         <v>MeanFreq_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P15" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyAccJerkMag-meanFreq()                      New Column Name: MeanFreq_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyAccJerkMag-meanFreq()     &gt;&gt;     MeanFreq_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="16" spans="2:16">
@@ -2187,8 +2191,8 @@
         <v>StdDev_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
       </c>
       <c r="P16" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyAccJerkMag-std()                      New Column Name: StdDev_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyAccJerkMag-std()     &gt;&gt;     StdDev_of_Magnitude_from_Body_Accelerometer_Jerk_freq</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -2222,8 +2226,8 @@
         <v>Mean_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
       </c>
       <c r="P17" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyGyroJerkMag-mean()                      New Column Name: Mean_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyGyroJerkMag-mean()     &gt;&gt;     Mean_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -2257,8 +2261,8 @@
         <v>MeanFreq_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
       </c>
       <c r="P18" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyGyroJerkMag-meanFreq()                      New Column Name: MeanFreq_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyGyroJerkMag-meanFreq()     &gt;&gt;     MeanFreq_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
       </c>
     </row>
     <row r="19" spans="2:16">
@@ -2292,8 +2296,8 @@
         <v>StdDev_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
       </c>
       <c r="P19" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyGyroJerkMag-std()                      New Column Name: StdDev_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyGyroJerkMag-std()     &gt;&gt;     StdDev_of_Magnitude_from_Body_Gyroscope_Jerk_freq</v>
       </c>
     </row>
     <row r="20" spans="2:16">
@@ -2327,8 +2331,8 @@
         <v>Mean_of_X_from_Body_Accelerometer_Jerk_time</v>
       </c>
       <c r="P20" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccJerk-mean()-X                      New Column Name: Mean_of_X_from_Body_Accelerometer_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccJerk-mean()-X     &gt;&gt;     Mean_of_X_from_Body_Accelerometer_Jerk_time</v>
       </c>
     </row>
     <row r="21" spans="2:16">
@@ -2362,8 +2366,8 @@
         <v>Mean_of_Y_from_Body_Accelerometer_Jerk_time</v>
       </c>
       <c r="P21" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccJerk-mean()-Y                      New Column Name: Mean_of_Y_from_Body_Accelerometer_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccJerk-mean()-Y     &gt;&gt;     Mean_of_Y_from_Body_Accelerometer_Jerk_time</v>
       </c>
     </row>
     <row r="22" spans="2:16">
@@ -2397,8 +2401,8 @@
         <v>Mean_of_Z_from_Body_Accelerometer_Jerk_time</v>
       </c>
       <c r="P22" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccJerk-mean()-Z                      New Column Name: Mean_of_Z_from_Body_Accelerometer_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccJerk-mean()-Z     &gt;&gt;     Mean_of_Z_from_Body_Accelerometer_Jerk_time</v>
       </c>
     </row>
     <row r="23" spans="2:16">
@@ -2432,8 +2436,8 @@
         <v>StdDev_of_X_from_Body_Accelerometer_Jerk_time</v>
       </c>
       <c r="P23" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccJerk-std()-X                      New Column Name: StdDev_of_X_from_Body_Accelerometer_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccJerk-std()-X     &gt;&gt;     StdDev_of_X_from_Body_Accelerometer_Jerk_time</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -2467,8 +2471,8 @@
         <v>StdDev_of_Y_from_Body_Accelerometer_Jerk_time</v>
       </c>
       <c r="P24" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccJerk-std()-Y                      New Column Name: StdDev_of_Y_from_Body_Accelerometer_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccJerk-std()-Y     &gt;&gt;     StdDev_of_Y_from_Body_Accelerometer_Jerk_time</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -2502,8 +2506,8 @@
         <v>StdDev_of_Z_from_Body_Accelerometer_Jerk_time</v>
       </c>
       <c r="P25" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccJerk-std()-Z                      New Column Name: StdDev_of_Z_from_Body_Accelerometer_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccJerk-std()-Z     &gt;&gt;     StdDev_of_Z_from_Body_Accelerometer_Jerk_time</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -2537,8 +2541,8 @@
         <v>Mean_of_Magnitude_from_Body_Accelerometer_Jerk_time</v>
       </c>
       <c r="P26" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccJerkMag-mean()                      New Column Name: Mean_of_Magnitude_from_Body_Accelerometer_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccJerkMag-mean()     &gt;&gt;     Mean_of_Magnitude_from_Body_Accelerometer_Jerk_time</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -2572,8 +2576,8 @@
         <v>StdDev_of_Magnitude_from_Body_Accelerometer_Jerk_time</v>
       </c>
       <c r="P27" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccJerkMag-std()                      New Column Name: StdDev_of_Magnitude_from_Body_Accelerometer_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccJerkMag-std()     &gt;&gt;     StdDev_of_Magnitude_from_Body_Accelerometer_Jerk_time</v>
       </c>
     </row>
     <row r="28" spans="2:16">
@@ -2607,8 +2611,8 @@
         <v>Mean_of_X_from_Body_Gyroscope_Jerk_time</v>
       </c>
       <c r="P28" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroJerk-mean()-X                      New Column Name: Mean_of_X_from_Body_Gyroscope_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroJerk-mean()-X     &gt;&gt;     Mean_of_X_from_Body_Gyroscope_Jerk_time</v>
       </c>
     </row>
     <row r="29" spans="2:16">
@@ -2642,8 +2646,8 @@
         <v>Mean_of_Y_from_Body_Gyroscope_Jerk_time</v>
       </c>
       <c r="P29" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroJerk-mean()-Y                      New Column Name: Mean_of_Y_from_Body_Gyroscope_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroJerk-mean()-Y     &gt;&gt;     Mean_of_Y_from_Body_Gyroscope_Jerk_time</v>
       </c>
     </row>
     <row r="30" spans="2:16">
@@ -2677,8 +2681,8 @@
         <v>Mean_of_Z_from_Body_Gyroscope_Jerk_time</v>
       </c>
       <c r="P30" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroJerk-mean()-Z                      New Column Name: Mean_of_Z_from_Body_Gyroscope_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroJerk-mean()-Z     &gt;&gt;     Mean_of_Z_from_Body_Gyroscope_Jerk_time</v>
       </c>
     </row>
     <row r="31" spans="2:16">
@@ -2712,8 +2716,8 @@
         <v>StdDev_of_X_from_Body_Gyroscope_Jerk_time</v>
       </c>
       <c r="P31" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroJerk-std()-X                      New Column Name: StdDev_of_X_from_Body_Gyroscope_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroJerk-std()-X     &gt;&gt;     StdDev_of_X_from_Body_Gyroscope_Jerk_time</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -2747,8 +2751,8 @@
         <v>StdDev_of_Y_from_Body_Gyroscope_Jerk_time</v>
       </c>
       <c r="P32" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroJerk-std()-Y                      New Column Name: StdDev_of_Y_from_Body_Gyroscope_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroJerk-std()-Y     &gt;&gt;     StdDev_of_Y_from_Body_Gyroscope_Jerk_time</v>
       </c>
     </row>
     <row r="33" spans="2:16">
@@ -2782,8 +2786,8 @@
         <v>StdDev_of_Z_from_Body_Gyroscope_Jerk_time</v>
       </c>
       <c r="P33" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroJerk-std()-Z                      New Column Name: StdDev_of_Z_from_Body_Gyroscope_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroJerk-std()-Z     &gt;&gt;     StdDev_of_Z_from_Body_Gyroscope_Jerk_time</v>
       </c>
     </row>
     <row r="34" spans="2:16">
@@ -2817,8 +2821,8 @@
         <v>Mean_of_Magnitude_from_Body_Gyroscope_Jerk_time</v>
       </c>
       <c r="P34" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroJerkMag-mean()                      New Column Name: Mean_of_Magnitude_from_Body_Gyroscope_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroJerkMag-mean()     &gt;&gt;     Mean_of_Magnitude_from_Body_Gyroscope_Jerk_time</v>
       </c>
     </row>
     <row r="35" spans="2:16">
@@ -2852,8 +2856,8 @@
         <v>StdDev_of_Magnitude_from_Body_Gyroscope_Jerk_time</v>
       </c>
       <c r="P35" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroJerkMag-std()                      New Column Name: StdDev_of_Magnitude_from_Body_Gyroscope_Jerk_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroJerkMag-std()     &gt;&gt;     StdDev_of_Magnitude_from_Body_Gyroscope_Jerk_time</v>
       </c>
     </row>
     <row r="36" spans="2:16">
@@ -2874,8 +2878,8 @@
         <v>104</v>
       </c>
       <c r="P36" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: Labels                      New Column Name: Activity_Measured</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>Labels     &gt;&gt;     Activity_Measured</v>
       </c>
     </row>
     <row r="37" spans="2:16">
@@ -2896,8 +2900,8 @@
         <v>103</v>
       </c>
       <c r="P37" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: Subject                      New Column Name: ID_Num_of_Subject</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>Subject     &gt;&gt;     ID_Num_of_Subject</v>
       </c>
     </row>
     <row r="38" spans="2:16">
@@ -2929,8 +2933,8 @@
         <v>Mean_of_X_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P38" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-mean()-X                      New Column Name: Mean_of_X_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-mean()-X     &gt;&gt;     Mean_of_X_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="39" spans="2:16">
@@ -2962,8 +2966,8 @@
         <v>Mean_of_Y_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P39" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-mean()-Y                      New Column Name: Mean_of_Y_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-mean()-Y     &gt;&gt;     Mean_of_Y_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="40" spans="2:16">
@@ -2995,8 +2999,8 @@
         <v>Mean_of_Z_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P40" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-mean()-Z                      New Column Name: Mean_of_Z_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-mean()-Z     &gt;&gt;     Mean_of_Z_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="41" spans="2:16">
@@ -3028,8 +3032,8 @@
         <v>MeanFreq_of_X_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P41" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-meanFreq()-X                      New Column Name: MeanFreq_of_X_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-meanFreq()-X     &gt;&gt;     MeanFreq_of_X_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="42" spans="2:16">
@@ -3061,8 +3065,8 @@
         <v>MeanFreq_of_Y_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P42" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-meanFreq()-Y                      New Column Name: MeanFreq_of_Y_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-meanFreq()-Y     &gt;&gt;     MeanFreq_of_Y_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="43" spans="2:16">
@@ -3094,8 +3098,8 @@
         <v>MeanFreq_of_Z_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P43" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-meanFreq()-Z                      New Column Name: MeanFreq_of_Z_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-meanFreq()-Z     &gt;&gt;     MeanFreq_of_Z_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="44" spans="2:16">
@@ -3127,8 +3131,8 @@
         <v>StdDev_of_X_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P44" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-std()-X                      New Column Name: StdDev_of_X_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-std()-X     &gt;&gt;     StdDev_of_X_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="45" spans="2:16">
@@ -3160,8 +3164,8 @@
         <v>StdDev_of_Y_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P45" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-std()-Y                      New Column Name: StdDev_of_Y_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-std()-Y     &gt;&gt;     StdDev_of_Y_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="46" spans="2:16">
@@ -3193,8 +3197,8 @@
         <v>StdDev_of_Z_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P46" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAcc-std()-Z                      New Column Name: StdDev_of_Z_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAcc-std()-Z     &gt;&gt;     StdDev_of_Z_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="47" spans="2:16">
@@ -3226,8 +3230,8 @@
         <v>Mean_of_Mag_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P47" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccMag-mean()                      New Column Name: Mean_of_Mag_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccMag-mean()     &gt;&gt;     Mean_of_Mag_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="48" spans="2:16">
@@ -3259,8 +3263,8 @@
         <v>MeanFreq_of_Mag_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P48" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccMag-meanFreq()                      New Column Name: MeanFreq_of_Mag_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccMag-meanFreq()     &gt;&gt;     MeanFreq_of_Mag_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="49" spans="2:16">
@@ -3292,8 +3296,8 @@
         <v>StdDev_of_Mag_from_Body_Accelerometer_freq</v>
       </c>
       <c r="P49" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyAccMag-std()                      New Column Name: StdDev_of_Mag_from_Body_Accelerometer_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyAccMag-std()     &gt;&gt;     StdDev_of_Mag_from_Body_Accelerometer_freq</v>
       </c>
     </row>
     <row r="50" spans="2:16">
@@ -3325,8 +3329,8 @@
         <v>Mean_of_Mag_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P50" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyGyroMag-mean()                      New Column Name: Mean_of_Mag_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyGyroMag-mean()     &gt;&gt;     Mean_of_Mag_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="51" spans="2:16">
@@ -3358,8 +3362,8 @@
         <v>MeanFreq_of_Mag_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P51" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyGyroMag-meanFreq()                      New Column Name: MeanFreq_of_Mag_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyGyroMag-meanFreq()     &gt;&gt;     MeanFreq_of_Mag_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="52" spans="2:16">
@@ -3391,8 +3395,8 @@
         <v>StdDev_of_Mag_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P52" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyBodyGyroMag-std()                      New Column Name: StdDev_of_Mag_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyBodyGyroMag-std()     &gt;&gt;     StdDev_of_Mag_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="53" spans="2:16">
@@ -3424,8 +3428,8 @@
         <v>Mean_of_X_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P53" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-mean()-X                      New Column Name: Mean_of_X_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-mean()-X     &gt;&gt;     Mean_of_X_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="54" spans="2:16">
@@ -3457,8 +3461,8 @@
         <v>Mean_of_Y_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P54" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-mean()-Y                      New Column Name: Mean_of_Y_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-mean()-Y     &gt;&gt;     Mean_of_Y_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="55" spans="2:16">
@@ -3490,8 +3494,8 @@
         <v>Mean_of_Z_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P55" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-mean()-Z                      New Column Name: Mean_of_Z_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-mean()-Z     &gt;&gt;     Mean_of_Z_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="56" spans="2:16">
@@ -3523,8 +3527,8 @@
         <v>MeanFreq_of_X_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P56" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-meanFreq()-X                      New Column Name: MeanFreq_of_X_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-meanFreq()-X     &gt;&gt;     MeanFreq_of_X_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="57" spans="2:16">
@@ -3556,8 +3560,8 @@
         <v>MeanFreq_of_Y_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P57" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-meanFreq()-Y                      New Column Name: MeanFreq_of_Y_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-meanFreq()-Y     &gt;&gt;     MeanFreq_of_Y_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="58" spans="2:16">
@@ -3589,8 +3593,8 @@
         <v>MeanFreq_of_Z_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P58" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-meanFreq()-Z                      New Column Name: MeanFreq_of_Z_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-meanFreq()-Z     &gt;&gt;     MeanFreq_of_Z_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="59" spans="2:16">
@@ -3622,8 +3626,8 @@
         <v>StdDev_of_X_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P59" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-std()-X                      New Column Name: StdDev_of_X_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-std()-X     &gt;&gt;     StdDev_of_X_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="60" spans="2:16">
@@ -3655,8 +3659,8 @@
         <v>StdDev_of_Y_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P60" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-std()-Y                      New Column Name: StdDev_of_Y_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-std()-Y     &gt;&gt;     StdDev_of_Y_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="61" spans="2:16">
@@ -3688,8 +3692,8 @@
         <v>StdDev_of_Z_from_Body_Gyroscope_freq</v>
       </c>
       <c r="P61" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: fBodyGyro-std()-Z                      New Column Name: StdDev_of_Z_from_Body_Gyroscope_freq</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>fBodyGyro-std()-Z     &gt;&gt;     StdDev_of_Z_from_Body_Gyroscope_freq</v>
       </c>
     </row>
     <row r="62" spans="2:16">
@@ -3721,8 +3725,8 @@
         <v>Mean_of_X_from_Body_Accelerometer_time</v>
       </c>
       <c r="P62" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAcc-mean()-X                      New Column Name: Mean_of_X_from_Body_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAcc-mean()-X     &gt;&gt;     Mean_of_X_from_Body_Accelerometer_time</v>
       </c>
     </row>
     <row r="63" spans="2:16">
@@ -3754,8 +3758,8 @@
         <v>Mean_of_Y_from_Body_Accelerometer_time</v>
       </c>
       <c r="P63" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAcc-mean()-Y                      New Column Name: Mean_of_Y_from_Body_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAcc-mean()-Y     &gt;&gt;     Mean_of_Y_from_Body_Accelerometer_time</v>
       </c>
     </row>
     <row r="64" spans="2:16">
@@ -3787,8 +3791,8 @@
         <v>Mean_of_Z_from_Body_Accelerometer_time</v>
       </c>
       <c r="P64" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAcc-mean()-Z                      New Column Name: Mean_of_Z_from_Body_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAcc-mean()-Z     &gt;&gt;     Mean_of_Z_from_Body_Accelerometer_time</v>
       </c>
     </row>
     <row r="65" spans="2:16">
@@ -3820,8 +3824,8 @@
         <v>StdDev_of_X_from_Body_Accelerometer_time</v>
       </c>
       <c r="P65" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAcc-std()-X                      New Column Name: StdDev_of_X_from_Body_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAcc-std()-X     &gt;&gt;     StdDev_of_X_from_Body_Accelerometer_time</v>
       </c>
     </row>
     <row r="66" spans="2:16">
@@ -3853,8 +3857,8 @@
         <v>StdDev_of_Y_from_Body_Accelerometer_time</v>
       </c>
       <c r="P66" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAcc-std()-Y                      New Column Name: StdDev_of_Y_from_Body_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAcc-std()-Y     &gt;&gt;     StdDev_of_Y_from_Body_Accelerometer_time</v>
       </c>
     </row>
     <row r="67" spans="2:16">
@@ -3886,8 +3890,8 @@
         <v>StdDev_of_Z_from_Body_Accelerometer_time</v>
       </c>
       <c r="P67" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAcc-std()-Z                      New Column Name: StdDev_of_Z_from_Body_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAcc-std()-Z     &gt;&gt;     StdDev_of_Z_from_Body_Accelerometer_time</v>
       </c>
     </row>
     <row r="68" spans="2:16">
@@ -3919,8 +3923,8 @@
         <v>Mean_of_Mag_from_Body_Accelerometer_time</v>
       </c>
       <c r="P68" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccMag-mean()                      New Column Name: Mean_of_Mag_from_Body_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccMag-mean()     &gt;&gt;     Mean_of_Mag_from_Body_Accelerometer_time</v>
       </c>
     </row>
     <row r="69" spans="2:16">
@@ -3952,8 +3956,8 @@
         <v>StdDev_of_Mag_from_Body_Accelerometer_time</v>
       </c>
       <c r="P69" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyAccMag-std()                      New Column Name: StdDev_of_Mag_from_Body_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyAccMag-std()     &gt;&gt;     StdDev_of_Mag_from_Body_Accelerometer_time</v>
       </c>
     </row>
     <row r="70" spans="2:16">
@@ -3985,8 +3989,8 @@
         <v>Mean_of_X_from_Body_Gyroscope_time</v>
       </c>
       <c r="P70" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyro-mean()-X                      New Column Name: Mean_of_X_from_Body_Gyroscope_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyro-mean()-X     &gt;&gt;     Mean_of_X_from_Body_Gyroscope_time</v>
       </c>
     </row>
     <row r="71" spans="2:16">
@@ -4018,8 +4022,8 @@
         <v>Mean_of_Y_from_Body_Gyroscope_time</v>
       </c>
       <c r="P71" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyro-mean()-Y                      New Column Name: Mean_of_Y_from_Body_Gyroscope_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyro-mean()-Y     &gt;&gt;     Mean_of_Y_from_Body_Gyroscope_time</v>
       </c>
     </row>
     <row r="72" spans="2:16">
@@ -4051,8 +4055,8 @@
         <v>Mean_of_Z_from_Body_Gyroscope_time</v>
       </c>
       <c r="P72" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyro-mean()-Z                      New Column Name: Mean_of_Z_from_Body_Gyroscope_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyro-mean()-Z     &gt;&gt;     Mean_of_Z_from_Body_Gyroscope_time</v>
       </c>
     </row>
     <row r="73" spans="2:16">
@@ -4084,8 +4088,8 @@
         <v>StdDev_of_X_from_Body_Gyroscope_time</v>
       </c>
       <c r="P73" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyro-std()-X                      New Column Name: StdDev_of_X_from_Body_Gyroscope_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyro-std()-X     &gt;&gt;     StdDev_of_X_from_Body_Gyroscope_time</v>
       </c>
     </row>
     <row r="74" spans="2:16">
@@ -4117,8 +4121,8 @@
         <v>StdDev_of_Y_from_Body_Gyroscope_time</v>
       </c>
       <c r="P74" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyro-std()-Y                      New Column Name: StdDev_of_Y_from_Body_Gyroscope_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyro-std()-Y     &gt;&gt;     StdDev_of_Y_from_Body_Gyroscope_time</v>
       </c>
     </row>
     <row r="75" spans="2:16">
@@ -4150,8 +4154,8 @@
         <v>StdDev_of_Z_from_Body_Gyroscope_time</v>
       </c>
       <c r="P75" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyro-std()-Z                      New Column Name: StdDev_of_Z_from_Body_Gyroscope_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyro-std()-Z     &gt;&gt;     StdDev_of_Z_from_Body_Gyroscope_time</v>
       </c>
     </row>
     <row r="76" spans="2:16">
@@ -4183,8 +4187,8 @@
         <v>Mean_of_Mag_from_Body_Gyroscope_time</v>
       </c>
       <c r="P76" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroMag-mean()                      New Column Name: Mean_of_Mag_from_Body_Gyroscope_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroMag-mean()     &gt;&gt;     Mean_of_Mag_from_Body_Gyroscope_time</v>
       </c>
     </row>
     <row r="77" spans="2:16">
@@ -4216,8 +4220,8 @@
         <v>StdDev_of_Mag_from_Body_Gyroscope_time</v>
       </c>
       <c r="P77" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tBodyGyroMag-std()                      New Column Name: StdDev_of_Mag_from_Body_Gyroscope_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tBodyGyroMag-std()     &gt;&gt;     StdDev_of_Mag_from_Body_Gyroscope_time</v>
       </c>
     </row>
     <row r="78" spans="2:16">
@@ -4249,8 +4253,8 @@
         <v>Mean_of_X_from_Gravity_Accelerometer_time</v>
       </c>
       <c r="P78" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tGravityAcc-mean()-X                      New Column Name: Mean_of_X_from_Gravity_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tGravityAcc-mean()-X     &gt;&gt;     Mean_of_X_from_Gravity_Accelerometer_time</v>
       </c>
     </row>
     <row r="79" spans="2:16">
@@ -4282,8 +4286,8 @@
         <v>Mean_of_Y_from_Gravity_Accelerometer_time</v>
       </c>
       <c r="P79" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tGravityAcc-mean()-Y                      New Column Name: Mean_of_Y_from_Gravity_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tGravityAcc-mean()-Y     &gt;&gt;     Mean_of_Y_from_Gravity_Accelerometer_time</v>
       </c>
     </row>
     <row r="80" spans="2:16">
@@ -4315,8 +4319,8 @@
         <v>Mean_of_Z_from_Gravity_Accelerometer_time</v>
       </c>
       <c r="P80" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tGravityAcc-mean()-Z                      New Column Name: Mean_of_Z_from_Gravity_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tGravityAcc-mean()-Z     &gt;&gt;     Mean_of_Z_from_Gravity_Accelerometer_time</v>
       </c>
     </row>
     <row r="81" spans="2:16">
@@ -4348,8 +4352,8 @@
         <v>StdDev_of_X_from_Gravity_Accelerometer_time</v>
       </c>
       <c r="P81" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tGravityAcc-std()-X                      New Column Name: StdDev_of_X_from_Gravity_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tGravityAcc-std()-X     &gt;&gt;     StdDev_of_X_from_Gravity_Accelerometer_time</v>
       </c>
     </row>
     <row r="82" spans="2:16">
@@ -4381,8 +4385,8 @@
         <v>StdDev_of_Y_from_Gravity_Accelerometer_time</v>
       </c>
       <c r="P82" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tGravityAcc-std()-Y                      New Column Name: StdDev_of_Y_from_Gravity_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tGravityAcc-std()-Y     &gt;&gt;     StdDev_of_Y_from_Gravity_Accelerometer_time</v>
       </c>
     </row>
     <row r="83" spans="2:16">
@@ -4414,8 +4418,8 @@
         <v>StdDev_of_Z_from_Gravity_Accelerometer_time</v>
       </c>
       <c r="P83" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tGravityAcc-std()-Z                      New Column Name: StdDev_of_Z_from_Gravity_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tGravityAcc-std()-Z     &gt;&gt;     StdDev_of_Z_from_Gravity_Accelerometer_time</v>
       </c>
     </row>
     <row r="84" spans="2:16">
@@ -4447,8 +4451,8 @@
         <v>Mean_of_Mag_from_Gravity_Accelerometer_time</v>
       </c>
       <c r="P84" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tGravityAccMag-mean()                      New Column Name: Mean_of_Mag_from_Gravity_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tGravityAccMag-mean()     &gt;&gt;     Mean_of_Mag_from_Gravity_Accelerometer_time</v>
       </c>
     </row>
     <row r="85" spans="2:16">
@@ -4480,8 +4484,8 @@
         <v>StdDev_of_Mag_from_Gravity_Accelerometer_time</v>
       </c>
       <c r="P85" t="str">
-        <f>"Old Column Name: "&amp;Table2[[#This Row],[Current]]&amp;"                      New Column Name: "&amp;Table2[[#This Row],[New]]</f>
-        <v>Old Column Name: tGravityAccMag-std()                      New Column Name: StdDev_of_Mag_from_Gravity_Accelerometer_time</v>
+        <f>Table2[[#This Row],[Current]]&amp;"     &gt;&gt;     "&amp;Table2[[#This Row],[New]]</f>
+        <v>tGravityAccMag-std()     &gt;&gt;     StdDev_of_Mag_from_Gravity_Accelerometer_time</v>
       </c>
     </row>
   </sheetData>

</xml_diff>